<commit_message>
aggiunti riferimeti anno scorso per soglia
</commit_message>
<xml_diff>
--- a/site/DB/stat_asta_22-23.xlsx
+++ b/site/DB/stat_asta_22-23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G.Aurilio\Source\Repos\susyleague\site\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9442AFF-3AA8-43A4-AF19-FC777C6A38E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6254B0-35E7-4FA1-8299-2B1CB7507D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1620" windowWidth="29040" windowHeight="15840" xr2:uid="{B1301CEE-C6F7-4B6C-8C62-DAB2662A3075}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1301CEE-C6F7-4B6C-8C62-DAB2662A3075}"/>
   </bookViews>
   <sheets>
     <sheet name="acquisti" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>C</t>
   </si>
@@ -120,25 +120,67 @@
     <t>F6</t>
   </si>
   <si>
-    <t>Colonna1</t>
-  </si>
-  <si>
-    <t>Colonna2</t>
-  </si>
-  <si>
-    <t>Colonna3</t>
-  </si>
-  <si>
-    <t>Colonna4</t>
-  </si>
-  <si>
-    <t>Colonna5</t>
-  </si>
-  <si>
-    <t>Colonna6</t>
-  </si>
-  <si>
-    <t>F7</t>
+    <t>&gt;=25</t>
+  </si>
+  <si>
+    <t>&gt;=20</t>
+  </si>
+  <si>
+    <t>&gt;=10</t>
+  </si>
+  <si>
+    <t>&gt;=5</t>
+  </si>
+  <si>
+    <t>&gt;=2</t>
+  </si>
+  <si>
+    <t>=1</t>
+  </si>
+  <si>
+    <t>&gt;=15</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>&gt;=40</t>
+  </si>
+  <si>
+    <t>&lt;4</t>
+  </si>
+  <si>
+    <t>&gt;=100</t>
+  </si>
+  <si>
+    <t>&gt;=75</t>
+  </si>
+  <si>
+    <t>&gt;=35</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>361</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>852</t>
   </si>
 </sst>
 </file>
@@ -195,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +274,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -626,11 +674,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -689,16 +817,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -708,15 +827,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -777,48 +887,114 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="13">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -826,7 +1002,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -843,15 +1019,15 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -868,10 +1044,113 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -888,35 +1167,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B324A95-4A60-4E10-813B-6775CBE86277}" name="Tabella3" displayName="Tabella3" ref="N1:Z5" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D10F997-B230-4506-BC9B-1D7308CAACB7}" name="Tabella1" displayName="Tabella1" ref="N2:Z9" totalsRowShown="0" headerRowDxfId="12">
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{7C6222CF-F5A0-43F0-96E2-5D26FE028E6C}" name="Colonna1" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{EB6FFD46-B474-4F1D-AD67-83F238C222EB}" name="F1" dataDxfId="11">
-      <calculatedColumnFormula>SUMIFS($B3:$B19,$A3:$A19,"&lt;100",$A3:$A19,"&gt;=35")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{4BC5ADE5-90E8-40A9-A3A9-98EAA7F43663}" name="Colonna2" dataDxfId="5">
-      <calculatedColumnFormula>SUMIFS($C3:$C19,$A3:$A19,"&lt;100",$A3:$A19,"&gt;=35")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{E2B117E8-C712-4383-98AD-E49A6287D676}" name="F2" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{25BB68F2-255A-4C83-8DDC-2C70964BD181}" name="Colonna3" dataDxfId="4">
-      <calculatedColumnFormula>SUMIFS($C3:$C19,$A3:$A19,"&lt;100",$A3:$A19,"&gt;=35")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{EC1B0509-2E4A-4942-9931-793892A5CBA1}" name="F3" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{F4B9D9D4-3ABD-4A08-B525-4D167D1F48F9}" name="Colonna4" dataDxfId="3">
-      <calculatedColumnFormula>SUMIFS($C3:$C19,$A3:$A19,"&lt;100",$A3:$A19,"&gt;=35")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{37F4E309-FF3E-4040-9B8E-CF41395549C8}" name="F4" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{F57CE56E-64D1-4CBE-85C5-A608D623BE59}" name="Colonna5" dataDxfId="2">
-      <calculatedColumnFormula>SUMIFS($C3:$C19,$A3:$A19,"&lt;100",$A3:$A19,"&gt;=35")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{32F46FB7-83FD-4B1F-990F-E28063B2C073}" name="F5" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{4055249D-680A-4761-A921-C3AA395FF4DD}" name="Colonna6" dataDxfId="1">
-      <calculatedColumnFormula>SUMIFS($C3:$C19,$A3:$A19,"&lt;100",$A3:$A19,"&gt;=35")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{2E090F76-A0EC-4AFD-AE26-29DE5DCB4F93}" name="F6" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{CBBD19EA-C084-4B9F-886B-D89EFF5AB0AF}" name="F7" dataDxfId="6">
-      <calculatedColumnFormula>SUM(F22:F25)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{7EB88912-7D52-4D44-90B0-15294C5492CF}" name="F1"/>
+    <tableColumn id="2" xr3:uid="{FEA393AE-8327-4CD6-8B02-010865A568D3}" name="&gt;=35" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{1ED55ED0-7CBC-41C2-9CAB-4927B9FC97BC}" name="5" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{608FBD14-1921-42DA-9B6C-650A8BD51217}" name="216" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{FCB619CF-8079-42E8-902F-DC526B5E7BAC}" name="&gt;=25" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{B87DFED1-D232-481C-BD3C-A2DFA609538C}" name="3" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{ACF635F2-9407-4D6C-AA26-3C7C9F847479}" name="103" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{2B537632-7EE9-438A-A56A-A7C790649364}" name="&gt;=40" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{0600DD23-5079-465C-93F1-5A45953D852B}" name="8" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{0E85CF20-82B0-458F-99BC-0D374C6B43F0}" name="361" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{7FBE005E-F283-4D5D-9394-F7AC30832E2A}" name="&gt;=100" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{8927CF94-2A18-4946-A871-CE306400C27D}" name="6" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{4EBD979A-9D83-4172-9715-1B76BA325D95}" name="852" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1221,183 +1486,153 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BED273F-183C-45F7-A44D-19E0582FA9DA}">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="26" width="7.21875" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" customWidth="1"/>
+    <col min="14" max="26" width="7.44140625" customWidth="1"/>
+    <col min="27" max="27" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="24" t="s">
+      <c r="E1" s="71"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="24" t="s">
+      <c r="H1" s="71"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="36"/>
-      <c r="N1" t="s">
+      <c r="K1" s="71"/>
+      <c r="L1" s="30"/>
+      <c r="O1" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="68"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" s="68"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="69"/>
+    </row>
+    <row r="2" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="49"/>
+      <c r="G2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="49"/>
+      <c r="J2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="24"/>
+      <c r="N2" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y1" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="26"/>
-      <c r="N2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="27">
-        <f>SUMIFS($B3:$B19,$A3:$A19,"&lt;100",$A3:$A19,"&gt;=35")</f>
-        <v>5</v>
-      </c>
-      <c r="P2" s="27">
-        <f t="shared" ref="P2:P5" si="0">SUMIFS($C3:$C19,$A3:$A19,"&lt;100",$A3:$A19,"&gt;=35")</f>
-        <v>216</v>
-      </c>
-      <c r="Q2" s="27">
-        <f>SUMIFS($B3:$B19,$A3:$A19,"&lt;35",$A3:$A19,"&gt;=20")</f>
-        <v>2</v>
-      </c>
-      <c r="R2" s="27">
-        <f>SUMIFS($C3:$C19,$A3:$A19,"&lt;35",$A3:$A19,"&gt;=20")</f>
-        <v>50</v>
-      </c>
-      <c r="S2" s="27">
-        <f>SUMIFS($B3:$B19,$A3:$A19,"&lt;20",$A3:$A19,"&gt;=10")</f>
-        <v>3</v>
-      </c>
-      <c r="T2" s="27">
-        <f>SUMIFS($C3:$C19,$A3:$A19,"&lt;20",$A3:$A19,"&gt;=10")</f>
+      <c r="S2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="27">
-        <f>SUMIFS($B3:$B19,$A3:$A19,"&lt;10",$A3:$A19,"&gt;=5")</f>
-        <v>10</v>
-      </c>
-      <c r="V2" s="27">
-        <f>SUMIFS($C3:$C19,$A3:$A19,"&lt;10",$A3:$A19,"&gt;=5")</f>
-        <v>62</v>
-      </c>
-      <c r="W2" s="27">
-        <f>SUMIFS($B3:$B19,$A3:$A19,"&lt;5",$A3:$A19,"&gt;=2")</f>
-        <v>4</v>
-      </c>
-      <c r="X2" s="27">
-        <f>SUMIFS($C3:$C19,$A3:$A19,"&lt;5",$A3:$A19,"&gt;=2")</f>
-        <v>12</v>
-      </c>
-      <c r="Y2" s="27">
-        <f>SUMIFS($B3:$B19,$A3:$A19,"&lt;2",$A3:$A19,"&gt;=1")</f>
-        <v>13</v>
-      </c>
-      <c r="Z2" s="27">
-        <f>SUMIFS($C3:$C19,$A3:$A19,"&lt;2",$A3:$A19,"&gt;=1")</f>
-        <v>13</v>
+      <c r="T2" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" s="57" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20">
         <v>59</v>
       </c>
-      <c r="B3" s="50">
+      <c r="B3" s="44">
         <v>1</v>
       </c>
       <c r="C3" s="21">
         <f>B3*A3</f>
         <v>59</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="36">
         <v>49</v>
       </c>
-      <c r="E3" s="43">
-        <v>1</v>
-      </c>
-      <c r="F3" s="44">
+      <c r="E3" s="37">
+        <v>1</v>
+      </c>
+      <c r="F3" s="38">
         <f>E3*D3</f>
         <v>49</v>
       </c>
       <c r="G3" s="20">
         <v>51</v>
       </c>
-      <c r="H3" s="50">
+      <c r="H3" s="44">
         <v>1</v>
       </c>
       <c r="I3" s="21">
@@ -1407,584 +1642,719 @@
       <c r="J3" s="20">
         <v>176</v>
       </c>
-      <c r="K3" s="50">
+      <c r="K3" s="44">
         <v>1</v>
       </c>
       <c r="L3" s="21">
         <f>K3*J3</f>
         <v>176</v>
       </c>
-      <c r="N3" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="27">
-        <f>SUMIFS($E3:$E26,$D3:$D26,"&lt;100",$D3:$D26,"&gt;=25")</f>
-        <v>3</v>
-      </c>
-      <c r="P3" s="27">
-        <f>SUMIFS($F3:$F26,$D3:$D26,"&lt;100",$D3:$D26,"&gt;=25")</f>
-        <v>103</v>
-      </c>
-      <c r="Q3" s="27">
-        <f>SUMIFS($E3:$E26,$D3:$D26,"&lt;25",$D3:$D26,"&gt;=20")</f>
+      <c r="N3" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="54">
+        <f>SUMIFS($B$3:$B$19,$A$3:$A$19,"&lt;35",$A$3:$A$19,"&gt;=20")</f>
+        <v>2</v>
+      </c>
+      <c r="Q3" s="59">
+        <f>SUMIFS($C$3:$C$19,$A$3:$A$19,"&lt;35",$A$3:$A$19,"&gt;=20")</f>
+        <v>50</v>
+      </c>
+      <c r="R3" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="52">
+        <f>SUMIFS($E$3:$E$26,$D$3:$D$26,"&lt;25",$D$3:$D$26,"&gt;=20")</f>
         <v>5</v>
       </c>
-      <c r="R3" s="27">
-        <f>SUMIFS($F3:$F26,$D3:$D26,"&lt;25",$D3:$D26,"&gt;=20")</f>
+      <c r="T3" s="57">
+        <f>SUMIFS($F$3:$F$26,$D$3:$D$26,"&lt;25",$D$3:$D$26,"&gt;=20")</f>
         <v>102</v>
       </c>
-      <c r="S3" s="27">
-        <f>SUMIFS($E3:$E26,$D3:$D26,"&lt;20",$D3:$D26,"&gt;=15")</f>
+      <c r="U3" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="54">
+        <f>SUMIFS($H$3:$H$34,$G$3:$G$34,"&lt;40",$G$3:$G$34,"&gt;=25")</f>
         <v>8</v>
       </c>
-      <c r="T3" s="27">
-        <f>SUMIFS($F3:$F26,$D3:$D26,"&lt;20",$D3:$D26,"&gt;=15")</f>
-        <v>141</v>
-      </c>
-      <c r="U3" s="27">
-        <f>SUMIFS($E3:$E26,$D3:$D26,"&lt;15",$D3:$D26,"&gt;=10")</f>
-        <v>14</v>
-      </c>
-      <c r="V3" s="27">
-        <f>SUMIFS($F3:$F26,$D3:$D26,"&lt;15",$D3:$D26,"&gt;=10")</f>
-        <v>161</v>
-      </c>
-      <c r="W3" s="27">
-        <f>SUMIFS($E3:$E26,$D3:$D26,"&lt;10",$D3:$D26,"&gt;=4")</f>
-        <v>43</v>
-      </c>
-      <c r="X3" s="27">
-        <f>SUMIFS($F3:$F26,$D3:$D26,"&lt;10",$D3:$D26,"&gt;=4")</f>
-        <v>240</v>
-      </c>
-      <c r="Y3" s="27">
-        <f>SUMIFS($E3:$E26,$D3:$D26,"&lt;4",$D3:$D26,"&gt;=1")</f>
-        <v>19</v>
-      </c>
-      <c r="Z3" s="27">
-        <f>SUMIFS($F3:$F26,$D3:$D26,"&lt;4",$D3:$D26,"&gt;=1")</f>
-        <v>44</v>
+      <c r="W3" s="59">
+        <f>SUMIFS($I$3:$I$34,$G$3:$G$34,"&lt;40",$G$3:$G$34,"&gt;=25")</f>
+        <v>235</v>
+      </c>
+      <c r="X3" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="52">
+        <f>SUMIFS($K$3:$K$43,$J$3:$J$43,"&lt;100",$J$3:$J$43,"&gt;=75")</f>
+        <v>5</v>
+      </c>
+      <c r="Z3" s="57">
+        <f>SUMIFS($L$3:$L$43,$J$3:$J$43,"&lt;100",$J$3:$J$43,"&gt;=75")</f>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>44</v>
       </c>
-      <c r="B4" s="39">
-        <v>1</v>
-      </c>
-      <c r="C4" s="38">
-        <f t="shared" ref="C4:C19" si="1">B4*A4</f>
+      <c r="B4" s="33">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32">
+        <f t="shared" ref="C4:C19" si="0">B4*A4</f>
         <v>44</v>
       </c>
       <c r="D4" s="22">
         <v>28</v>
       </c>
-      <c r="E4" s="45">
-        <v>1</v>
-      </c>
-      <c r="F4" s="46">
-        <f t="shared" ref="F4:F26" si="2">E4*D4</f>
+      <c r="E4" s="39">
+        <v>1</v>
+      </c>
+      <c r="F4" s="40">
+        <f t="shared" ref="F4:F26" si="1">E4*D4</f>
         <v>28</v>
       </c>
       <c r="G4" s="7">
         <v>50</v>
       </c>
-      <c r="H4" s="39">
-        <v>1</v>
-      </c>
-      <c r="I4" s="38">
-        <f t="shared" ref="I4:I34" si="3">H4*G4</f>
+      <c r="H4" s="33">
+        <v>1</v>
+      </c>
+      <c r="I4" s="32">
+        <f t="shared" ref="I4:I34" si="2">H4*G4</f>
         <v>50</v>
       </c>
       <c r="J4" s="7">
         <v>163</v>
       </c>
-      <c r="K4" s="39">
-        <v>1</v>
-      </c>
-      <c r="L4" s="38">
-        <f t="shared" ref="L4:L43" si="4">K4*J4</f>
+      <c r="K4" s="33">
+        <v>1</v>
+      </c>
+      <c r="L4" s="32">
+        <f t="shared" ref="L4:L43" si="3">K4*J4</f>
         <v>163</v>
       </c>
-      <c r="N4" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="27">
-        <f>SUMIFS($H3:$H34,$G3:$G34,"&lt;100",$G3:$G34,"&gt;=40")</f>
+      <c r="N4" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="53">
+        <f>SUMIFS($B$3:$B$19,$A$3:$A$19,"&lt;20",$A$3:$A$19,"&gt;=10")</f>
+        <v>3</v>
+      </c>
+      <c r="Q4" s="60">
+        <f>SUMIFS($C$3:$C$19,$A$3:$A$19,"&lt;20",$A$3:$A$19,"&gt;=10")</f>
+        <v>42</v>
+      </c>
+      <c r="R4" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="53">
+        <f>SUMIFS($E$3:$E$26,$D$3:$D$26,"&lt;20",$D$3:$D$26,"&gt;=15")</f>
         <v>8</v>
       </c>
-      <c r="P4" s="27">
-        <f>SUMIFS($I3:$I34,$G3:$G34,"&lt;100",$G3:$G34,"&gt;=40")</f>
-        <v>361</v>
-      </c>
-      <c r="Q4" s="27">
-        <f>SUMIFS($H3:$H34,$G3:$G34,"&lt;40",$G3:$G34,"&gt;=25")</f>
+      <c r="T4" s="60">
+        <f>SUMIFS($F$3:$F$26,$D$3:$D$26,"&lt;20",$D$3:$D$26,"&gt;=15")</f>
+        <v>141</v>
+      </c>
+      <c r="U4" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" s="53">
+        <f>SUMIFS($H$3:$H$34,$G$3:$G$34,"&lt;25",$G$3:$G$34,"&gt;=15")</f>
+        <v>24</v>
+      </c>
+      <c r="W4" s="60">
+        <f>SUMIFS($I$3:$I$34,$G$3:$G$34,"&lt;25",$G$3:$G$34,"&gt;=15")</f>
+        <v>449</v>
+      </c>
+      <c r="X4" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4" s="53">
+        <f>SUMIFS($K$3:$K$43,$J$3:$J$43,"&lt;75",$J$3:$J$43,"&gt;=40")</f>
         <v>8</v>
       </c>
-      <c r="R4" s="27">
-        <f>SUMIFS($I3:$I34,$G3:$G34,"&lt;40",$G3:$G34,"&gt;=25")</f>
-        <v>235</v>
-      </c>
-      <c r="S4" s="27">
-        <f>SUMIFS($H3:$H34,$G3:$G34,"&lt;25",$G3:$G34,"&gt;=15")</f>
-        <v>24</v>
-      </c>
-      <c r="T4" s="27">
-        <f>SUMIFS($I3:$I34,$G3:$G34,"&lt;25",$G3:$G34,"&gt;=15")</f>
-        <v>449</v>
-      </c>
-      <c r="U4" s="27">
-        <f>SUMIFS($H3:$H34,$G3:$G34,"&lt;15",$G3:$G34,"&gt;=10")</f>
-        <v>9</v>
-      </c>
-      <c r="V4" s="27">
-        <f>SUMIFS($I3:$I34,$G3:$G34,"&lt;15",$G3:$G34,"&gt;=10")</f>
-        <v>110</v>
-      </c>
-      <c r="W4" s="27">
-        <f>SUMIFS($H3:$H34,$G3:$G34,"&lt;10",$G3:$G34,"&gt;=4")</f>
-        <v>20</v>
-      </c>
-      <c r="X4" s="27">
-        <f>SUMIFS($I3:$I34,$G3:$G34,"&lt;10",$G3:$G34,"&gt;=4")</f>
-        <v>118</v>
-      </c>
-      <c r="Y4" s="27">
-        <f>SUMIFS($H3:$H34,$G3:$G34,"&lt;4",$G3:$G34,"&gt;=1")</f>
-        <v>45</v>
-      </c>
-      <c r="Z4" s="27">
-        <f>SUMIFS($I3:$I34,$G3:$G34,"&lt;4",$G3:$G34,"&gt;=1")</f>
-        <v>66</v>
+      <c r="Z4" s="60">
+        <f>SUMIFS($L$3:$L$43,$J$3:$J$43,"&lt;70",$J$3:$J$43,"&gt;=40")</f>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>42</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="31">
         <v>1</v>
       </c>
       <c r="C5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="D5" s="5">
         <v>26</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="31">
         <v>1</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="G5" s="5">
         <v>48</v>
       </c>
-      <c r="H5" s="37">
+      <c r="H5" s="31">
         <v>1</v>
       </c>
       <c r="I5" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="J5" s="5">
         <v>160</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="31">
         <v>1</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="N5" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="O5" s="27">
-        <f>SUMIFS($K3:$K43,$J3:$J43,"&lt;200",$J3:$J43,"&gt;=100")</f>
-        <v>6</v>
-      </c>
-      <c r="P5" s="27">
-        <f>SUMIFS($L3:$L43,$J3:$J43,"&lt;200",$J3:$J43,"&gt;=100")</f>
-        <v>852</v>
-      </c>
-      <c r="Q5" s="27">
-        <f>SUMIFS($K3:$K43,$J3:$J43,"&lt;100",$J3:$J43,"&gt;=75")</f>
-        <v>5</v>
-      </c>
-      <c r="R5" s="27">
-        <f>SUMIFS($L3:$L43,$J3:$J43,"&lt;100",$J3:$J43,"&gt;=75")</f>
-        <v>410</v>
-      </c>
-      <c r="S5" s="27">
-        <f>SUMIFS($K3:$K43,$J3:$J43,"&lt;75",$J3:$J43,"&gt;=40")</f>
-        <v>8</v>
-      </c>
-      <c r="T5" s="27">
-        <f>SUMIFS($L3:$L43,$J3:$J43,"&lt;75",$J3:$J43,"&gt;=40")</f>
-        <v>407</v>
-      </c>
-      <c r="U5" s="27">
-        <f>SUMIFS($K3:$K43,$J3:$J43,"&lt;40",$J3:$J43,"&gt;=15")</f>
+      <c r="N5" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="54">
+        <f>SUMIFS($B$3:$B$19,$A$3:$A$19,"&lt;10",$A$3:$A$19,"&gt;=5")</f>
+        <v>10</v>
+      </c>
+      <c r="Q5" s="59">
+        <f>SUMIFS($C$3:$C$19,$A$3:$A$19,"&lt;10",$A$3:$A$19,"&gt;=5")</f>
+        <v>62</v>
+      </c>
+      <c r="R5" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="52">
+        <f>SUMIFS($E$3:$E$26,$D$3:$D$26,"&lt;15",$D$3:$D$26,"&gt;=10")</f>
+        <v>14</v>
+      </c>
+      <c r="T5" s="57">
+        <f>SUMIFS($F$3:$F$26,$D$3:$D$26,"&lt;15",$D$3:$D$26,"&gt;=10")</f>
+        <v>161</v>
+      </c>
+      <c r="U5" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" s="54">
+        <f>SUMIFS($H$3:$H$34,$G$3:$G$34,"&lt;15",$G$3:$G$34,"&gt;=10")</f>
+        <v>9</v>
+      </c>
+      <c r="W5" s="59">
+        <f>SUMIFS($I$3:$I$34,$G$3:$G$34,"&lt;15",$G$3:$G$34,"&gt;=10")</f>
+        <v>110</v>
+      </c>
+      <c r="X5" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y5" s="52">
+        <f>SUMIFS($K$3:$K$43,$J$3:$J$43,"&lt;40",$J$3:$J$43,"&gt;=15")</f>
         <v>13</v>
       </c>
-      <c r="V5" s="27">
-        <f>SUMIFS($L3:$L43,$J3:$J43,"&lt;40",$J3:$J43,"&gt;=15")</f>
+      <c r="Z5" s="57">
+        <f>SUMIFS($L$3:$L$43,$J$3:$J$43,"&lt;40",$J$3:$J$43,"&gt;=15")</f>
         <v>327</v>
-      </c>
-      <c r="W5" s="27">
-        <f>SUMIFS($K3:$K43,$J3:$J43,"&lt;15",$J3:$J43,"&gt;=4")</f>
-        <v>23</v>
-      </c>
-      <c r="X5" s="27">
-        <f>SUMIFS($L3:$L43,$J3:$J43,"&lt;15",$J3:$J43,"&gt;=4")</f>
-        <v>203</v>
-      </c>
-      <c r="Y5" s="27">
-        <f>SUMIFS($K3:$K43,$J3:$J43,"&lt;4",$J3:$J43,"&gt;=1")</f>
-        <v>32</v>
-      </c>
-      <c r="Z5" s="27">
-        <f>SUMIFS($L3:$L43,$J3:$J43,"&lt;4",$J3:$J43,"&gt;=1")</f>
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>36</v>
       </c>
-      <c r="B6" s="39">
-        <v>1</v>
-      </c>
-      <c r="C6" s="38">
-        <f t="shared" si="1"/>
+      <c r="B6" s="33">
+        <v>1</v>
+      </c>
+      <c r="C6" s="32">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="D6" s="7">
         <v>21</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="33">
         <v>2</v>
       </c>
-      <c r="F6" s="38">
-        <f t="shared" si="2"/>
+      <c r="F6" s="32">
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="G6" s="7">
         <v>47</v>
       </c>
-      <c r="H6" s="39">
-        <v>1</v>
-      </c>
-      <c r="I6" s="38">
-        <f t="shared" si="3"/>
+      <c r="H6" s="33">
+        <v>1</v>
+      </c>
+      <c r="I6" s="32">
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="J6" s="7">
         <v>130</v>
       </c>
-      <c r="K6" s="39">
-        <v>1</v>
-      </c>
-      <c r="L6" s="38">
-        <f t="shared" si="4"/>
+      <c r="K6" s="33">
+        <v>1</v>
+      </c>
+      <c r="L6" s="32">
+        <f t="shared" si="3"/>
         <v>130</v>
+      </c>
+      <c r="N6" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="53">
+        <f>SUMIFS($B$3:$B$19,$A$3:$A$19,"&lt;5",$A$3:$A$19,"&gt;=2")</f>
+        <v>4</v>
+      </c>
+      <c r="Q6" s="60">
+        <f>SUMIFS($C$3:$C$19,$A$3:$A$19,"&lt;5",$A$3:$A$19,"&gt;=2")</f>
+        <v>12</v>
+      </c>
+      <c r="R6" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="53">
+        <f>SUMIFS($E$3:$E$26,$D$3:$D$26,"&lt;10",$D$3:$D$26,"&gt;=4")</f>
+        <v>43</v>
+      </c>
+      <c r="T6" s="60">
+        <f>SUMIFS($F$3:$F$26,$D$3:$D$26,"&lt;10",$D$3:$D$26,"&gt;=4")</f>
+        <v>240</v>
+      </c>
+      <c r="U6" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" s="53">
+        <f>SUMIFS($H$3:$H$34,$G$3:$G$34,"&lt;10",$G$3:$G$34,"&gt;=4")</f>
+        <v>20</v>
+      </c>
+      <c r="W6" s="60">
+        <f>SUMIFS($I$3:$I$34,$G$3:$G$34,"&lt;10",$G$3:$G$34,"&gt;=4")</f>
+        <v>118</v>
+      </c>
+      <c r="X6" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" s="53">
+        <f>SUMIFS($K$3:$K$43,$J$3:$J$43,"&lt;15",$J$3:$J$43,"&gt;=4")</f>
+        <v>23</v>
+      </c>
+      <c r="Z6" s="60">
+        <f>SUMIFS($L$3:$L$43,$J$3:$J$43,"&lt;15",$J$3:$J$43,"&gt;=4")</f>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>35</v>
       </c>
-      <c r="B7" s="49">
-        <v>1</v>
-      </c>
-      <c r="C7" s="48">
-        <f t="shared" si="1"/>
+      <c r="B7" s="43">
+        <v>1</v>
+      </c>
+      <c r="C7" s="42">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="D7" s="12">
         <v>20</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="43">
         <v>3</v>
       </c>
       <c r="F7" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G7" s="5">
         <v>44</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="31">
         <v>1</v>
       </c>
       <c r="I7" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J7" s="5">
         <v>120</v>
       </c>
-      <c r="K7" s="37">
+      <c r="K7" s="31">
         <v>1</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>120</v>
+      </c>
+      <c r="N7" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="62">
+        <f>SUMIFS($B$3:$B$19,$A$3:$A$19,"&lt;2",$A$3:$A$19,"&gt;=1")</f>
+        <v>13</v>
+      </c>
+      <c r="Q7" s="63">
+        <f>SUMIFS($C15:$C31,$A15:$A31,"&lt;2",$A15:$A31,"&gt;=1")</f>
+        <v>13</v>
+      </c>
+      <c r="R7" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="65">
+        <f>SUMIFS($E$3:$E$26,$D$3:$D$26,"&lt;4",$D$3:$D$26,"&gt;=1")</f>
+        <v>19</v>
+      </c>
+      <c r="T7" s="66">
+        <f>SUMIFS($F$3:$F$26,$D$3:$D$26,"&lt;4",$D$3:$D$26,"&gt;=1")</f>
+        <v>44</v>
+      </c>
+      <c r="U7" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="V7" s="62">
+        <f>SUMIFS($H$3:$H$34,$G$3:$G$34,"&lt;4",$G$3:$G$34,"&gt;=1")</f>
+        <v>45</v>
+      </c>
+      <c r="W7" s="63">
+        <f>SUMIFS($I$3:$I$34,$G$3:$G$34,"&lt;4",$G$3:$G$34,"&gt;=1")</f>
+        <v>66</v>
+      </c>
+      <c r="X7" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y7" s="65">
+        <f>SUMIFS($K$3:$K$43,$J$3:$J$43,"&lt;4",$J$3:$J$43,"&gt;=1")</f>
+        <v>32</v>
+      </c>
+      <c r="Z7" s="66">
+        <f>SUMIFS($L$3:$L$43,$J$3:$J$43,"&lt;4",$J$3:$J$43,"&gt;=1")</f>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19">
         <v>25</v>
       </c>
-      <c r="B8" s="51">
+      <c r="B8" s="45">
         <v>2</v>
       </c>
-      <c r="C8" s="52">
-        <f t="shared" si="1"/>
+      <c r="C8" s="46">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="D8" s="22">
         <v>19</v>
       </c>
-      <c r="E8" s="45">
+      <c r="E8" s="39">
         <v>3</v>
       </c>
-      <c r="F8" s="46">
-        <f t="shared" si="2"/>
+      <c r="F8" s="40">
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="G8" s="7">
         <v>41</v>
       </c>
-      <c r="H8" s="39">
-        <v>1</v>
-      </c>
-      <c r="I8" s="38">
-        <f t="shared" si="3"/>
+      <c r="H8" s="33">
+        <v>1</v>
+      </c>
+      <c r="I8" s="32">
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="J8" s="23">
         <v>103</v>
       </c>
-      <c r="K8" s="47">
-        <v>1</v>
-      </c>
-      <c r="L8" s="48">
-        <f t="shared" si="4"/>
+      <c r="K8" s="41">
+        <v>1</v>
+      </c>
+      <c r="L8" s="42">
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="51"/>
+      <c r="Y8" s="51"/>
+      <c r="Z8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>15</v>
       </c>
-      <c r="B9" s="50">
+      <c r="B9" s="44">
         <v>1</v>
       </c>
       <c r="C9" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D9" s="5">
         <v>18</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="31">
         <v>2</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="G9" s="12">
         <v>40</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="43">
         <v>2</v>
       </c>
       <c r="I9" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="J9" s="20">
         <v>92</v>
       </c>
-      <c r="K9" s="50">
+      <c r="K9" s="44">
         <v>1</v>
       </c>
       <c r="L9" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="51"/>
+      <c r="W9" s="51"/>
+      <c r="X9" s="51"/>
+      <c r="Y9" s="51"/>
+      <c r="Z9" s="51"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>14</v>
       </c>
-      <c r="B10" s="39">
-        <v>1</v>
-      </c>
-      <c r="C10" s="38">
-        <f t="shared" si="1"/>
+      <c r="B10" s="33">
+        <v>1</v>
+      </c>
+      <c r="C10" s="32">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="D10" s="7">
         <v>17</v>
       </c>
-      <c r="E10" s="39">
-        <v>1</v>
-      </c>
-      <c r="F10" s="38">
-        <f t="shared" si="2"/>
+      <c r="E10" s="33">
+        <v>1</v>
+      </c>
+      <c r="F10" s="32">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G10" s="22">
         <v>39</v>
       </c>
-      <c r="H10" s="45">
-        <v>1</v>
-      </c>
-      <c r="I10" s="46">
-        <f t="shared" si="3"/>
+      <c r="H10" s="39">
+        <v>1</v>
+      </c>
+      <c r="I10" s="40">
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="J10" s="7">
         <v>86</v>
       </c>
-      <c r="K10" s="39">
-        <v>1</v>
-      </c>
-      <c r="L10" s="38">
-        <f t="shared" si="4"/>
+      <c r="K10" s="33">
+        <v>1</v>
+      </c>
+      <c r="L10" s="32">
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="51"/>
+      <c r="W10" s="51"/>
+      <c r="X10" s="51"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="51"/>
     </row>
     <row r="11" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>13</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="43">
         <v>1</v>
       </c>
       <c r="C11" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="D11" s="5">
         <v>16</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="31">
         <v>1</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G11" s="5">
         <v>32</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="31">
         <v>1</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="J11" s="5">
         <v>80</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="31">
         <v>1</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="51"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="51"/>
+      <c r="X11" s="51"/>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22">
         <v>9</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="39">
         <v>2</v>
       </c>
-      <c r="C12" s="46">
-        <f t="shared" si="1"/>
+      <c r="C12" s="40">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D12" s="23">
         <v>15</v>
       </c>
-      <c r="E12" s="47">
-        <v>1</v>
-      </c>
-      <c r="F12" s="48">
-        <f t="shared" si="2"/>
+      <c r="E12" s="41">
+        <v>1</v>
+      </c>
+      <c r="F12" s="42">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G12" s="7">
         <v>30</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="33">
         <v>2</v>
       </c>
-      <c r="I12" s="38">
-        <f t="shared" si="3"/>
+      <c r="I12" s="32">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="J12" s="7">
         <v>77</v>
       </c>
-      <c r="K12" s="39">
-        <v>1</v>
-      </c>
-      <c r="L12" s="38">
-        <f t="shared" si="4"/>
+      <c r="K12" s="33">
+        <v>1</v>
+      </c>
+      <c r="L12" s="32">
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
+      <c r="W12" s="51"/>
     </row>
     <row r="13" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>7</v>
       </c>
-      <c r="B13" s="37">
+      <c r="B13" s="31">
         <v>1</v>
       </c>
       <c r="C13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D13" s="20">
         <v>14</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="44">
         <v>1</v>
       </c>
       <c r="F13" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G13" s="12">
         <v>26</v>
       </c>
-      <c r="H13" s="49">
+      <c r="H13" s="43">
         <v>4</v>
       </c>
       <c r="I13" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>104</v>
       </c>
       <c r="J13" s="12">
         <v>75</v>
       </c>
-      <c r="K13" s="49">
+      <c r="K13" s="43">
         <v>1</v>
       </c>
       <c r="L13" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
     </row>
@@ -1992,83 +2362,84 @@
       <c r="A14" s="7">
         <v>6</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="33">
         <v>2</v>
       </c>
-      <c r="C14" s="38">
-        <f t="shared" si="1"/>
+      <c r="C14" s="32">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="D14" s="7">
         <v>13</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="33">
         <v>3</v>
       </c>
-      <c r="F14" s="38">
-        <f t="shared" si="2"/>
+      <c r="F14" s="32">
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="G14" s="22">
         <v>24</v>
       </c>
-      <c r="H14" s="45">
+      <c r="H14" s="39">
         <v>3</v>
       </c>
-      <c r="I14" s="46">
-        <f t="shared" si="3"/>
+      <c r="I14" s="40">
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="J14" s="22">
         <v>62</v>
       </c>
-      <c r="K14" s="45">
-        <v>1</v>
-      </c>
-      <c r="L14" s="46">
-        <f t="shared" si="4"/>
+      <c r="K14" s="39">
+        <v>1</v>
+      </c>
+      <c r="L14" s="40">
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
+      <c r="Z14" s="51"/>
     </row>
     <row r="15" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>5</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="43">
         <v>5</v>
       </c>
       <c r="C15" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="D15" s="5">
         <v>12</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="31">
         <v>3</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="G15" s="5">
         <v>23</v>
       </c>
-      <c r="H15" s="37">
+      <c r="H15" s="31">
         <v>1</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="J15" s="5">
         <v>61</v>
       </c>
-      <c r="K15" s="37">
+      <c r="K15" s="31">
         <v>1</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
     </row>
@@ -2076,41 +2447,41 @@
       <c r="A16" s="22">
         <v>4</v>
       </c>
-      <c r="B16" s="45">
-        <v>1</v>
-      </c>
-      <c r="C16" s="46">
-        <f t="shared" si="1"/>
+      <c r="B16" s="39">
+        <v>1</v>
+      </c>
+      <c r="C16" s="40">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D16" s="7">
         <v>11</v>
       </c>
-      <c r="E16" s="39">
+      <c r="E16" s="33">
         <v>2</v>
       </c>
-      <c r="F16" s="38">
-        <f t="shared" si="2"/>
+      <c r="F16" s="32">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G16" s="7">
         <v>21</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="33">
         <v>4</v>
       </c>
-      <c r="I16" s="38">
-        <f t="shared" si="3"/>
+      <c r="I16" s="32">
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="J16" s="7">
         <v>58</v>
       </c>
-      <c r="K16" s="39">
-        <v>1</v>
-      </c>
-      <c r="L16" s="38">
-        <f t="shared" si="4"/>
+      <c r="K16" s="33">
+        <v>1</v>
+      </c>
+      <c r="L16" s="32">
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -2118,41 +2489,41 @@
       <c r="A17" s="5">
         <v>3</v>
       </c>
-      <c r="B17" s="37">
+      <c r="B17" s="31">
         <v>2</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D17" s="12">
         <v>10</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="43">
         <v>5</v>
       </c>
       <c r="F17" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="G17" s="5">
         <v>20</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="31">
         <v>2</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="J17" s="5">
         <v>57</v>
       </c>
-      <c r="K17" s="37">
+      <c r="K17" s="31">
         <v>1</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
     </row>
@@ -2160,750 +2531,754 @@
       <c r="A18" s="23">
         <v>2</v>
       </c>
-      <c r="B18" s="47">
-        <v>1</v>
-      </c>
-      <c r="C18" s="48">
-        <f t="shared" si="1"/>
+      <c r="B18" s="41">
+        <v>1</v>
+      </c>
+      <c r="C18" s="42">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D18" s="20">
         <v>9</v>
       </c>
-      <c r="E18" s="50">
+      <c r="E18" s="44">
         <v>3</v>
       </c>
       <c r="F18" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="G18" s="5">
         <v>18</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="31">
         <v>3</v>
       </c>
       <c r="I18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="J18" s="5">
         <v>43</v>
       </c>
-      <c r="K18" s="37">
+      <c r="K18" s="31">
         <v>2</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="42">
-        <v>1</v>
-      </c>
-      <c r="B19" s="43">
+      <c r="A19" s="36">
+        <v>1</v>
+      </c>
+      <c r="B19" s="37">
         <v>13</v>
       </c>
-      <c r="C19" s="44">
-        <f t="shared" si="1"/>
+      <c r="C19" s="38">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="D19" s="7">
         <v>8</v>
       </c>
-      <c r="E19" s="39">
+      <c r="E19" s="33">
         <v>2</v>
       </c>
-      <c r="F19" s="38">
-        <f t="shared" si="2"/>
+      <c r="F19" s="32">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G19" s="7">
         <v>17</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="33">
         <v>3</v>
       </c>
-      <c r="I19" s="38">
-        <f t="shared" si="3"/>
+      <c r="I19" s="32">
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="J19" s="7">
         <v>42</v>
       </c>
-      <c r="K19" s="39">
-        <v>1</v>
-      </c>
-      <c r="L19" s="38">
-        <f t="shared" si="4"/>
+      <c r="K19" s="33">
+        <v>1</v>
+      </c>
+      <c r="L19" s="32">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="40"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="31"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="5">
         <v>7</v>
       </c>
-      <c r="E20" s="37">
+      <c r="E20" s="31">
         <v>8</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="G20" s="5">
         <v>16</v>
       </c>
-      <c r="H20" s="37">
+      <c r="H20" s="31">
         <v>5</v>
       </c>
       <c r="I20" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="J20" s="12">
         <v>41</v>
       </c>
-      <c r="K20" s="49">
+      <c r="K20" s="43">
         <v>1</v>
       </c>
       <c r="L20" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="29"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="7">
         <v>6</v>
       </c>
-      <c r="E21" s="39">
+      <c r="E21" s="33">
         <v>7</v>
       </c>
-      <c r="F21" s="38">
-        <f t="shared" si="2"/>
+      <c r="F21" s="32">
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="G21" s="23">
         <v>15</v>
       </c>
-      <c r="H21" s="47">
+      <c r="H21" s="41">
         <v>3</v>
       </c>
-      <c r="I21" s="48">
-        <f t="shared" si="3"/>
+      <c r="I21" s="42">
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="J21" s="22">
         <v>33</v>
       </c>
-      <c r="K21" s="45">
+      <c r="K21" s="39">
         <v>2</v>
       </c>
-      <c r="L21" s="46">
-        <f t="shared" si="4"/>
+      <c r="L21" s="40">
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="30"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="5">
         <v>5</v>
       </c>
-      <c r="E22" s="37">
+      <c r="E22" s="31">
         <v>7</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="G22" s="20">
         <v>14</v>
       </c>
-      <c r="H22" s="50">
+      <c r="H22" s="44">
         <v>1</v>
       </c>
       <c r="I22" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J22" s="5">
         <v>31</v>
       </c>
-      <c r="K22" s="37">
+      <c r="K22" s="31">
         <v>1</v>
       </c>
       <c r="L22" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="31"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="23">
         <v>4</v>
       </c>
-      <c r="E23" s="47">
+      <c r="E23" s="41">
         <v>16</v>
       </c>
-      <c r="F23" s="48">
-        <f t="shared" si="2"/>
+      <c r="F23" s="42">
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="G23" s="7">
         <v>13</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="33">
         <v>5</v>
       </c>
-      <c r="I23" s="38">
-        <f t="shared" si="3"/>
+      <c r="I23" s="32">
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="J23" s="7">
         <v>30</v>
       </c>
-      <c r="K23" s="39">
+      <c r="K23" s="33">
         <v>2</v>
       </c>
-      <c r="L23" s="38">
-        <f t="shared" si="4"/>
+      <c r="L23" s="32">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="29"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="17">
         <v>3</v>
       </c>
-      <c r="E24" s="56">
+      <c r="E24" s="50">
         <v>8</v>
       </c>
       <c r="F24" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="G24" s="5">
         <v>11</v>
       </c>
-      <c r="H24" s="37">
+      <c r="H24" s="31">
         <v>1</v>
       </c>
       <c r="I24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="J24" s="5">
         <v>27</v>
       </c>
-      <c r="K24" s="37">
+      <c r="K24" s="31">
         <v>1</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="29"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="7">
         <v>2</v>
       </c>
-      <c r="E25" s="39">
+      <c r="E25" s="33">
         <v>9</v>
       </c>
-      <c r="F25" s="38">
-        <f t="shared" si="2"/>
+      <c r="F25" s="32">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="G25" s="23">
         <v>10</v>
       </c>
-      <c r="H25" s="47">
+      <c r="H25" s="41">
         <v>2</v>
       </c>
-      <c r="I25" s="48">
-        <f t="shared" si="3"/>
+      <c r="I25" s="42">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="J25" s="7">
         <v>25</v>
       </c>
-      <c r="K25" s="39">
-        <v>1</v>
-      </c>
-      <c r="L25" s="38">
-        <f t="shared" si="4"/>
+      <c r="K25" s="33">
+        <v>1</v>
+      </c>
+      <c r="L25" s="32">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="29"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="12">
         <v>1</v>
       </c>
-      <c r="E26" s="49">
+      <c r="E26" s="43">
         <v>2</v>
       </c>
       <c r="F26" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G26" s="20">
         <v>9</v>
       </c>
-      <c r="H26" s="50">
+      <c r="H26" s="44">
         <v>1</v>
       </c>
       <c r="I26" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J26" s="5">
         <v>23</v>
       </c>
-      <c r="K26" s="37">
+      <c r="K26" s="31">
         <v>1</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="31"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="5">
         <v>8</v>
       </c>
-      <c r="H27" s="37">
+      <c r="H27" s="31">
         <v>1</v>
       </c>
       <c r="I27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="J27" s="5">
         <v>22</v>
       </c>
-      <c r="K27" s="37">
+      <c r="K27" s="31">
         <v>1</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="29"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="29"/>
+      <c r="F28" s="26"/>
       <c r="G28" s="7">
         <v>7</v>
       </c>
-      <c r="H28" s="39">
+      <c r="H28" s="33">
         <v>5</v>
       </c>
-      <c r="I28" s="38">
-        <f t="shared" si="3"/>
+      <c r="I28" s="32">
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="J28" s="7">
         <v>20</v>
       </c>
-      <c r="K28" s="39">
-        <v>1</v>
-      </c>
-      <c r="L28" s="38">
-        <f t="shared" si="4"/>
+      <c r="K28" s="33">
+        <v>1</v>
+      </c>
+      <c r="L28" s="32">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="29"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="29"/>
+      <c r="F29" s="26"/>
       <c r="G29" s="5">
         <v>6</v>
       </c>
-      <c r="H29" s="37">
+      <c r="H29" s="31">
         <v>5</v>
       </c>
       <c r="I29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="J29" s="5">
         <v>19</v>
       </c>
-      <c r="K29" s="37">
+      <c r="K29" s="31">
         <v>1</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="29"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="30"/>
+      <c r="F30" s="27"/>
       <c r="G30" s="7">
         <v>5</v>
       </c>
-      <c r="H30" s="39">
+      <c r="H30" s="33">
         <v>4</v>
       </c>
-      <c r="I30" s="38">
-        <f t="shared" si="3"/>
+      <c r="I30" s="32">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="J30" s="23">
         <v>17</v>
       </c>
-      <c r="K30" s="47">
+      <c r="K30" s="41">
         <v>2</v>
       </c>
-      <c r="L30" s="48">
-        <f t="shared" si="4"/>
+      <c r="L30" s="42">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="29"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
-      <c r="F31" s="31"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12">
         <v>4</v>
       </c>
-      <c r="H31" s="49">
+      <c r="H31" s="43">
         <v>4</v>
       </c>
       <c r="I31" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J31" s="20">
         <v>14</v>
       </c>
-      <c r="K31" s="50">
+      <c r="K31" s="44">
         <v>1</v>
       </c>
       <c r="L31" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="29"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="29"/>
+      <c r="F32" s="26"/>
       <c r="G32" s="22">
         <v>3</v>
       </c>
-      <c r="H32" s="45">
+      <c r="H32" s="39">
         <v>7</v>
       </c>
-      <c r="I32" s="46">
-        <f t="shared" si="3"/>
+      <c r="I32" s="40">
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="J32" s="7">
         <v>13</v>
       </c>
-      <c r="K32" s="39">
+      <c r="K32" s="33">
         <v>2</v>
       </c>
-      <c r="L32" s="38">
-        <f t="shared" si="4"/>
+      <c r="L32" s="32">
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="29"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="29"/>
+      <c r="F33" s="26"/>
       <c r="G33" s="5">
         <v>2</v>
       </c>
-      <c r="H33" s="37">
+      <c r="H33" s="31">
         <v>7</v>
       </c>
       <c r="I33" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J33" s="5">
         <v>12</v>
       </c>
-      <c r="K33" s="37">
+      <c r="K33" s="31">
         <v>3</v>
       </c>
       <c r="L33" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="29"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
-      <c r="F34" s="29"/>
+      <c r="F34" s="26"/>
       <c r="G34" s="23">
         <v>1</v>
       </c>
-      <c r="H34" s="47">
+      <c r="H34" s="41">
         <v>31</v>
       </c>
-      <c r="I34" s="48">
-        <f t="shared" si="3"/>
+      <c r="I34" s="42">
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="J34" s="7">
         <v>11</v>
       </c>
-      <c r="K34" s="39">
-        <v>1</v>
-      </c>
-      <c r="L34" s="38">
-        <f t="shared" si="4"/>
+      <c r="K34" s="33">
+        <v>1</v>
+      </c>
+      <c r="L34" s="32">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="29"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="57"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="51"/>
       <c r="J35" s="5">
         <v>10</v>
       </c>
-      <c r="K35" s="37">
+      <c r="K35" s="31">
         <v>3</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="29"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
-      <c r="F36" s="29"/>
+      <c r="F36" s="26"/>
       <c r="G36" s="8"/>
       <c r="H36" s="9"/>
-      <c r="I36" s="31"/>
+      <c r="I36" s="28"/>
       <c r="J36" s="7">
         <v>8</v>
       </c>
-      <c r="K36" s="39">
+      <c r="K36" s="33">
         <v>4</v>
       </c>
-      <c r="L36" s="38">
-        <f t="shared" si="4"/>
+      <c r="L36" s="32">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="29"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="29"/>
+      <c r="F37" s="26"/>
       <c r="G37" s="8"/>
       <c r="H37" s="9"/>
-      <c r="I37" s="29"/>
+      <c r="I37" s="26"/>
       <c r="J37" s="5">
         <v>7</v>
       </c>
-      <c r="K37" s="37">
+      <c r="K37" s="31">
         <v>3</v>
       </c>
       <c r="L37" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
-      <c r="C38" s="29"/>
+      <c r="C38" s="26"/>
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="29"/>
+      <c r="F38" s="26"/>
       <c r="G38" s="8"/>
       <c r="H38" s="9"/>
-      <c r="I38" s="29"/>
+      <c r="I38" s="26"/>
       <c r="J38" s="7">
         <v>6</v>
       </c>
-      <c r="K38" s="39">
+      <c r="K38" s="33">
         <v>4</v>
       </c>
-      <c r="L38" s="38">
-        <f t="shared" si="4"/>
+      <c r="L38" s="32">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="9"/>
-      <c r="C39" s="29"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="29"/>
+      <c r="F39" s="26"/>
       <c r="G39" s="8"/>
       <c r="H39" s="9"/>
-      <c r="I39" s="29"/>
+      <c r="I39" s="26"/>
       <c r="J39" s="5">
         <v>5</v>
       </c>
-      <c r="K39" s="37">
+      <c r="K39" s="31">
         <v>1</v>
       </c>
       <c r="L39" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
-      <c r="C40" s="29"/>
+      <c r="C40" s="26"/>
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="29"/>
+      <c r="F40" s="26"/>
       <c r="G40" s="8"/>
       <c r="H40" s="9"/>
-      <c r="I40" s="29"/>
+      <c r="I40" s="26"/>
       <c r="J40" s="23">
         <v>4</v>
       </c>
-      <c r="K40" s="47">
-        <v>1</v>
-      </c>
-      <c r="L40" s="48">
-        <f t="shared" si="4"/>
+      <c r="K40" s="41">
+        <v>1</v>
+      </c>
+      <c r="L40" s="42">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="9"/>
-      <c r="C41" s="29"/>
+      <c r="C41" s="26"/>
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="29"/>
+      <c r="F41" s="26"/>
       <c r="G41" s="8"/>
       <c r="H41" s="9"/>
-      <c r="I41" s="29"/>
+      <c r="I41" s="26"/>
       <c r="J41" s="17">
         <v>3</v>
       </c>
-      <c r="K41" s="56">
+      <c r="K41" s="50">
         <v>3</v>
       </c>
       <c r="L41" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
-      <c r="C42" s="29"/>
+      <c r="C42" s="26"/>
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="29"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="8"/>
       <c r="H42" s="9"/>
-      <c r="I42" s="29"/>
+      <c r="I42" s="26"/>
       <c r="J42" s="7">
         <v>2</v>
       </c>
-      <c r="K42" s="39">
+      <c r="K42" s="33">
         <v>6</v>
       </c>
-      <c r="L42" s="38">
-        <f t="shared" si="4"/>
+      <c r="L42" s="32">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="32"/>
+      <c r="C43" s="29"/>
       <c r="D43" s="10"/>
       <c r="E43" s="11"/>
-      <c r="F43" s="32"/>
+      <c r="F43" s="29"/>
       <c r="G43" s="10"/>
       <c r="H43" s="11"/>
-      <c r="I43" s="32"/>
+      <c r="I43" s="29"/>
       <c r="J43" s="5">
         <v>1</v>
       </c>
-      <c r="K43" s="37">
+      <c r="K43" s="31">
         <v>23</v>
       </c>
       <c r="L43" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="G1:H1"/>
+  <mergeCells count="8">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>